<commit_message>
chore: code and slide text cleanup
</commit_message>
<xml_diff>
--- a/officer_demo_cat_data.xlsx
+++ b/officer_demo_cat_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Documents\projects\automated-slide-deck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB283602-7A9D-42E2-AFBA-18509A7F4258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C0FA9-8FC8-40F9-9B79-2B4007BB6832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5064" yWindow="2040" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report_Params" sheetId="1" r:id="rId1"/>
-    <sheet name="Open CE graphic text" sheetId="2" r:id="rId2"/>
+    <sheet name="Summary text" sheetId="2" r:id="rId2"/>
     <sheet name="CEs by month type" sheetId="3" r:id="rId3"/>
     <sheet name="CE Grade" sheetId="4" r:id="rId4"/>
     <sheet name="CE Outcome" sheetId="7" r:id="rId5"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
-  <si>
-    <t>Report_Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <t>Start_Date</t>
   </si>
@@ -146,15 +143,9 @@
     <t>Claws out</t>
   </si>
   <si>
-    <t>Greater Toronto Area</t>
-  </si>
-  <si>
     <t>GTA</t>
   </si>
   <si>
-    <t>Report_Name_Short</t>
-  </si>
-  <si>
     <t>Closed without Outcome</t>
   </si>
   <si>
@@ -209,9 +200,6 @@
     <t>Hiss</t>
   </si>
   <si>
-    <t>1,128 Cat Encounters (CEs) in the Greater Toronto Area</t>
-  </si>
-  <si>
     <t>Tabby (506 CEs)</t>
   </si>
   <si>
@@ -248,15 +236,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>August was the peak month for CEs, but trends showed an increase in CEs in the second half of the year</t>
-  </si>
-  <si>
-    <t>41% of CEs resulted in a Positive Experience outcome, compared to 35% in the previous report</t>
-  </si>
-  <si>
-    <t>Purr, Meow, and Stretch were the most frequent actions for CEs resulting in a Positive Experience outcome</t>
-  </si>
-  <si>
     <t>Positive Experience 462</t>
   </si>
   <si>
@@ -279,6 +258,21 @@
   </si>
   <si>
     <t>Further Investigation Needed 28</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>41% of CEs resulted in a Positive Experience outcome, up from 35% previously</t>
+  </si>
+  <si>
+    <t>Purr, Meow, and Stretch were the most frequent cat actions during Positive Experience CEs</t>
+  </si>
+  <si>
+    <t>August was the peak month for CEs, with an increase in CEs in the second half of the year</t>
+  </si>
+  <si>
+    <t>1,128 CEs in the GTA from April 1, 2022 to March 31, 2023</t>
   </si>
 </sst>
 </file>
@@ -357,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -426,17 +420,6 @@
       <right style="medium">
         <color rgb="FFC0C0C0"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFC0C0C0"/>
-      </right>
       <top style="medium">
         <color rgb="FFC0C0C0"/>
       </top>
@@ -475,24 +458,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -524,7 +507,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -539,13 +522,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -556,6 +533,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,63 +752,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="22.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="7" customWidth="1"/>
-    <col min="5" max="27" width="8.6640625" style="7" customWidth="1"/>
-    <col min="28" max="16384" width="14.44140625" style="7"/>
+    <col min="1" max="1" width="22.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="7" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" style="7" customWidth="1"/>
+    <col min="27" max="16384" width="14.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="11">
+        <v>44652</v>
       </c>
       <c r="C2" s="11">
-        <v>44652</v>
-      </c>
-      <c r="D2" s="11">
         <v>45016</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="7" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="8" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="10" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="11" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="12" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1"/>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1"/>
+    <row r="3" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="4" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="6" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="7" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="8" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="9" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="10" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="12.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="12.75" customHeight="1"/>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1"/>
     <row r="19" ht="12.75" customHeight="1"/>
@@ -1823,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1835,32 +1809,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.75" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="12.75" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="12.75" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="12.75" customHeight="1"/>
@@ -2869,13 +2843,13 @@
   <dimension ref="A1:H994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.88671875" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" style="7" customWidth="1"/>
@@ -2887,40 +2861,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A1" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>51</v>
+      <c r="A1" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="F1" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="14">
         <v>38</v>
@@ -2936,13 +2910,13 @@
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="14">
         <v>43</v>
@@ -2960,13 +2934,13 @@
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="14">
         <v>24</v>
@@ -2984,13 +2958,13 @@
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="14">
         <v>29</v>
@@ -3007,13 +2981,13 @@
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A6" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="14">
         <v>32</v>
@@ -3033,13 +3007,13 @@
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A7" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>7</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="14">
         <v>31</v>
@@ -3055,13 +3029,13 @@
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="14">
         <v>54</v>
@@ -3079,13 +3053,13 @@
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A9" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="14">
         <v>29</v>
@@ -3103,13 +3077,13 @@
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A10" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="14">
         <v>38</v>
@@ -3125,13 +3099,13 @@
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A11" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>17</v>
       </c>
       <c r="D11" s="14">
         <v>44</v>
@@ -3149,13 +3123,13 @@
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A12" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>15</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="14">
         <v>76</v>
@@ -3173,13 +3147,13 @@
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="14">
         <v>68</v>
@@ -4177,7 +4151,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4186,7 +4160,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -4200,24 +4174,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" s="14">
         <v>73</v>
@@ -4234,7 +4208,7 @@
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B3" s="14">
         <v>68</v>
@@ -4251,7 +4225,7 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" s="14">
         <v>48</v>
@@ -4268,7 +4242,7 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B5" s="14">
         <v>11</v>
@@ -4283,7 +4257,7 @@
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6" s="14">
         <v>16</v>
@@ -5298,7 +5272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5312,21 +5286,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4">
         <v>462</v>
@@ -5334,10 +5308,10 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6">
         <v>278</v>
@@ -5345,10 +5319,10 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6">
         <v>110</v>
@@ -5356,10 +5330,10 @@
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6">
         <v>101</v>
@@ -5367,10 +5341,10 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C6" s="6">
         <v>75</v>
@@ -5378,10 +5352,10 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C7" s="6">
         <v>42</v>
@@ -5389,10 +5363,10 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C8" s="6">
         <v>32</v>
@@ -5400,10 +5374,10 @@
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C9" s="6">
         <v>28</v>
@@ -6425,21 +6399,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A1" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A2" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="14">
         <v>295</v>
@@ -6453,7 +6427,7 @@
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A3" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="14">
         <v>289</v>
@@ -6465,7 +6439,7 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="14">
         <v>87</v>
@@ -6479,7 +6453,7 @@
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5" s="14">
         <v>53</v>
@@ -6493,7 +6467,7 @@
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A6" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="14">
         <v>51</v>
@@ -6507,7 +6481,7 @@
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A7" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="14">
         <v>42</v>
@@ -6521,7 +6495,7 @@
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" s="14">
         <v>31</v>
@@ -6533,7 +6507,7 @@
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A9" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="14">
         <v>26</v>
@@ -6545,7 +6519,7 @@
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A10" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="14">
         <v>18</v>
@@ -6557,7 +6531,7 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A11" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="14">
         <v>7</v>
@@ -6571,7 +6545,7 @@
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A12" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="14">
         <v>6</v>
@@ -6583,7 +6557,7 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A13" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="14">
         <v>4</v>
@@ -6597,7 +6571,7 @@
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A14" s="16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" s="14">
         <v>2</v>
@@ -6611,7 +6585,7 @@
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A15" s="16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="15">
@@ -6623,7 +6597,7 @@
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A16" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="15">
@@ -6635,7 +6609,7 @@
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A17" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>

</xml_diff>

<commit_message>
fix: update data dates
</commit_message>
<xml_diff>
--- a/officer_demo_cat_data.xlsx
+++ b/officer_demo_cat_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Documents\projects\automated-slide-deck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JRIECK\Documents\git_projects\auto-slide-deck-officer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491C0FA9-8FC8-40F9-9B79-2B4007BB6832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46544E1B-911B-4FF8-B619-1671503F7FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="2040" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report_Params" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>End_Date</t>
   </si>
   <si>
-    <t>22-23</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -272,7 +269,10 @@
     <t>August was the peak month for CEs, with an increase in CEs in the second half of the year</t>
   </si>
   <si>
-    <t>1,128 CEs in the GTA from April 1, 2022 to March 31, 2023</t>
+    <t>1,128 CEs in the GTA from April 1, 2023 to March 31, 2024</t>
+  </si>
+  <si>
+    <t>23-24</t>
   </si>
 </sst>
 </file>
@@ -755,7 +755,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -769,7 +769,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -780,13 +780,13 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="11">
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="C2" s="11">
-        <v>45016</v>
+        <v>45382</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1"/>
@@ -1797,7 +1797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1809,32 +1809,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.75" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="12.75" customHeight="1">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="12.75" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="12.75" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="12.75" customHeight="1"/>
@@ -2843,7 +2843,7 @@
   <dimension ref="A1:H994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2862,39 +2862,39 @@
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A1" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>48</v>
-      </c>
       <c r="D1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A2" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="14">
         <v>38</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="3" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A3" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="14">
         <v>43</v>
@@ -2934,13 +2934,13 @@
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>3</v>
-      </c>
       <c r="C4" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="14">
         <v>24</v>
@@ -2958,13 +2958,13 @@
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A5" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>8</v>
       </c>
       <c r="D5" s="14">
         <v>29</v>
@@ -2981,13 +2981,13 @@
     </row>
     <row r="6" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A6" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="14">
         <v>32</v>
@@ -3007,13 +3007,13 @@
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A7" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="14">
         <v>31</v>
@@ -3029,13 +3029,13 @@
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B8" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>12</v>
       </c>
       <c r="D8" s="14">
         <v>54</v>
@@ -3053,13 +3053,13 @@
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A9" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="14">
         <v>29</v>
@@ -3077,13 +3077,13 @@
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A10" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="14">
         <v>38</v>
@@ -3099,13 +3099,13 @@
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A11" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>15</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>16</v>
       </c>
       <c r="D11" s="14">
         <v>44</v>
@@ -3123,13 +3123,13 @@
     </row>
     <row r="12" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A12" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="14">
         <v>76</v>
@@ -3147,13 +3147,13 @@
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
       <c r="A13" s="20" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="14">
         <v>68</v>
@@ -4174,24 +4174,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="14">
         <v>73</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="14">
         <v>68</v>
@@ -4225,7 +4225,7 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="14">
         <v>48</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="14">
         <v>11</v>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="14">
         <v>16</v>
@@ -5272,7 +5272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5286,21 +5286,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4">
         <v>462</v>
@@ -5308,10 +5308,10 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6">
         <v>278</v>
@@ -5319,10 +5319,10 @@
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6">
         <v>110</v>
@@ -5330,10 +5330,10 @@
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6">
         <v>101</v>
@@ -5341,10 +5341,10 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="6">
         <v>75</v>
@@ -5352,10 +5352,10 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="6">
         <v>42</v>
@@ -5363,10 +5363,10 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="6">
         <v>32</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="6">
         <v>28</v>
@@ -6399,21 +6399,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A1" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A2" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="14">
         <v>295</v>
@@ -6427,7 +6427,7 @@
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A3" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="14">
         <v>289</v>
@@ -6439,7 +6439,7 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="14">
         <v>87</v>
@@ -6453,7 +6453,7 @@
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="14">
         <v>53</v>
@@ -6467,7 +6467,7 @@
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A6" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="14">
         <v>51</v>
@@ -6481,7 +6481,7 @@
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A7" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="14">
         <v>42</v>
@@ -6495,7 +6495,7 @@
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="14">
         <v>31</v>
@@ -6507,7 +6507,7 @@
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A9" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="14">
         <v>26</v>
@@ -6519,7 +6519,7 @@
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A10" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="14">
         <v>18</v>
@@ -6531,7 +6531,7 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A11" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="14">
         <v>7</v>
@@ -6545,7 +6545,7 @@
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="14">
         <v>6</v>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A13" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="14">
         <v>4</v>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A14" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="14">
         <v>2</v>
@@ -6585,7 +6585,7 @@
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A15" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="15">
@@ -6597,7 +6597,7 @@
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A16" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="15">
@@ -6609,7 +6609,7 @@
     </row>
     <row r="17" spans="1:4" ht="12.75" customHeight="1" thickBot="1">
       <c r="A17" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>

</xml_diff>